<commit_message>
add word counter tool page
</commit_message>
<xml_diff>
--- a/tools.xlsx
+++ b/tools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\saas\toolcorehub-frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD23B30-C1E7-4DF7-A08D-886732CCC979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBC0399-C6CB-4D38-B7A8-ECFAE2ABF1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Tool name/Primary Keyword</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>http://localhost:3000/tools/remove-empty-lines</t>
+  </si>
+  <si>
+    <t>websitedev91</t>
   </si>
 </sst>
 </file>
@@ -385,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,9 +399,10 @@
     <col min="1" max="1" width="33.77734375" customWidth="1"/>
     <col min="2" max="2" width="32.21875" customWidth="1"/>
     <col min="3" max="3" width="40.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,12 +413,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>